<commit_message>
correct latex formatting of $
</commit_message>
<xml_diff>
--- a/data/datasets.xlsx
+++ b/data/datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liam/Dropbox/_Projects/Smil-Growth/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA2FC63-AF41-2541-92E0-F58924028315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CBE293-FD80-A04C-88CD-4EF3422B1AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1037,9 +1037,6 @@
     <t>World Bank (2018)</t>
   </si>
   <si>
-    <t>Growth and logistic outlook of GDBP (expression in international $2011) in four major economies - France, Japan, and the US since 1870, and China since 1950. Data from World Bank (2018).</t>
-  </si>
-  <si>
     <t>Per capita income (US)</t>
   </si>
   <si>
@@ -1134,6 +1131,9 @@
   </si>
   <si>
     <t>Logistic curve in early stages - fails with SSfpl. Smil fits asymmetric logistic</t>
+  </si>
+  <si>
+    <t>Growth and logistic outlook of GDBP (expression in international \$2011) in four major economies - France, Japan, and the US since 1870, and China since 1950. Data from World Bank (2018).</t>
   </si>
 </sst>
 </file>
@@ -1994,8 +1994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D63" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" topLeftCell="E63" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2014,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2029,16 +2029,16 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>358</v>
+      </c>
+      <c r="H1" t="s">
         <v>359</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>360</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>361</v>
-      </c>
-      <c r="J1" t="s">
-        <v>362</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
@@ -2055,13 +2055,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -2069,7 +2069,7 @@
         <v>148</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C3" t="s">
         <v>154</v>
@@ -2099,7 +2099,7 @@
         <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M3" t="s">
         <v>158</v>
@@ -2113,7 +2113,7 @@
         <v>149</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C4" t="s">
         <v>155</v>
@@ -2268,10 +2268,10 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M8" t="s">
         <v>181</v>
@@ -2282,7 +2282,7 @@
         <v>150</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C9" t="s">
         <v>176</v>
@@ -2326,7 +2326,7 @@
         <v>151</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C10" t="s">
         <v>177</v>
@@ -2370,7 +2370,7 @@
         <v>152</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C11" t="s">
         <v>178</v>
@@ -2414,7 +2414,7 @@
         <v>153</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C12" t="s">
         <v>179</v>
@@ -2444,7 +2444,7 @@
         <v>47</v>
       </c>
       <c r="L12" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M12" t="s">
         <v>181</v>
@@ -2993,13 +2993,13 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M27" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -3007,7 +3007,7 @@
         <v>65</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C28" t="s">
         <v>66</v>
@@ -3051,7 +3051,7 @@
         <v>70</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C29" t="s">
         <v>66</v>
@@ -3081,13 +3081,13 @@
         <v>245</v>
       </c>
       <c r="L29" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M29" t="s">
         <v>71</v>
       </c>
       <c r="N29" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -3361,13 +3361,13 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
@@ -3375,7 +3375,7 @@
         <v>98</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C38" t="s">
         <v>99</v>
@@ -3405,7 +3405,7 @@
         <v>263</v>
       </c>
       <c r="L38" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M38" t="s">
         <v>102</v>
@@ -3419,7 +3419,7 @@
         <v>104</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C39" t="s">
         <v>105</v>
@@ -3449,7 +3449,7 @@
         <v>263</v>
       </c>
       <c r="L39" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M39" t="s">
         <v>107</v>
@@ -3463,7 +3463,7 @@
         <v>109</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C40" t="s">
         <v>110</v>
@@ -3493,7 +3493,7 @@
         <v>263</v>
       </c>
       <c r="L40" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M40" t="s">
         <v>112</v>
@@ -3507,7 +3507,7 @@
         <v>113</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C41" t="s">
         <v>114</v>
@@ -3537,7 +3537,7 @@
         <v>263</v>
       </c>
       <c r="L41" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M41" t="s">
         <v>116</v>
@@ -3859,7 +3859,7 @@
         <v>147</v>
       </c>
       <c r="N49" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
@@ -3978,10 +3978,10 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M53" t="s">
         <v>273</v>
@@ -3992,7 +3992,7 @@
         <v>233</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C54" t="s">
         <v>270</v>
@@ -4036,7 +4036,7 @@
         <v>234</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C55" t="s">
         <v>271</v>
@@ -4153,10 +4153,10 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M58" t="s">
         <v>287</v>
@@ -4167,7 +4167,7 @@
         <v>237</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C59" t="s">
         <v>281</v>
@@ -4211,7 +4211,7 @@
         <v>238</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C60" t="s">
         <v>282</v>
@@ -4364,7 +4364,7 @@
         <v>295</v>
       </c>
       <c r="N63" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -4711,13 +4711,13 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M73" t="s">
-        <v>334</v>
+        <v>366</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
@@ -4725,7 +4725,7 @@
         <v>251</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C74" t="s">
         <v>328</v>
@@ -4758,7 +4758,7 @@
         <v>13</v>
       </c>
       <c r="M74" t="s">
-        <v>334</v>
+        <v>366</v>
       </c>
       <c r="N74" t="s">
         <v>327</v>
@@ -4769,7 +4769,7 @@
         <v>252</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C75" t="s">
         <v>329</v>
@@ -4802,7 +4802,7 @@
         <v>13</v>
       </c>
       <c r="M75" t="s">
-        <v>334</v>
+        <v>366</v>
       </c>
       <c r="N75" t="s">
         <v>327</v>
@@ -4813,7 +4813,7 @@
         <v>253</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C76" t="s">
         <v>330</v>
@@ -4846,7 +4846,7 @@
         <v>13</v>
       </c>
       <c r="M76" t="s">
-        <v>334</v>
+        <v>366</v>
       </c>
       <c r="N76" t="s">
         <v>327</v>
@@ -4857,7 +4857,7 @@
         <v>254</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C77" t="s">
         <v>331</v>
@@ -4890,7 +4890,7 @@
         <v>13</v>
       </c>
       <c r="M77" t="s">
-        <v>334</v>
+        <v>366</v>
       </c>
       <c r="N77" t="s">
         <v>327</v>
@@ -4898,13 +4898,13 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M78" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -4912,16 +4912,16 @@
         <v>255</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C79" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D79" t="s">
         <v>16</v>
       </c>
       <c r="E79" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F79" t="s">
         <v>333</v>
@@ -4945,10 +4945,10 @@
         <v>13</v>
       </c>
       <c r="M79" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N79" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -4956,16 +4956,16 @@
         <v>256</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C80" t="s">
+        <v>336</v>
+      </c>
+      <c r="D80" t="s">
+        <v>16</v>
+      </c>
+      <c r="E80" t="s">
         <v>337</v>
-      </c>
-      <c r="D80" t="s">
-        <v>16</v>
-      </c>
-      <c r="E80" t="s">
-        <v>338</v>
       </c>
       <c r="F80" t="s">
         <v>333</v>
@@ -4989,10 +4989,10 @@
         <v>13</v>
       </c>
       <c r="M80" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N80" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -5000,16 +5000,16 @@
         <v>257</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C81" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D81" t="s">
         <v>16</v>
       </c>
       <c r="E81" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F81" t="s">
         <v>333</v>
@@ -5033,10 +5033,10 @@
         <v>13</v>
       </c>
       <c r="M81" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N81" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -5044,16 +5044,16 @@
         <v>258</v>
       </c>
       <c r="C82" t="s">
+        <v>340</v>
+      </c>
+      <c r="D82" t="s">
+        <v>16</v>
+      </c>
+      <c r="E82" t="s">
         <v>341</v>
       </c>
-      <c r="D82" t="s">
-        <v>16</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>342</v>
-      </c>
-      <c r="F82" t="s">
-        <v>343</v>
       </c>
       <c r="G82">
         <v>1870</v>
@@ -5074,7 +5074,7 @@
         <v>13</v>
       </c>
       <c r="M82" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -5120,10 +5120,10 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M84" t="s">
         <v>204</v>
@@ -5134,7 +5134,7 @@
         <v>190</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C85" t="s">
         <v>202</v>
@@ -5178,7 +5178,7 @@
         <v>191</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C86" t="s">
         <v>203</v>

</xml_diff>